<commit_message>
[Add] SOS 포탄 구현 [Update] 풀링 적용 중
</commit_message>
<xml_diff>
--- a/Assets/ExcelDatas/SkillData.xlsx
+++ b/Assets/ExcelDatas/SkillData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\Project_Advence-main\Assets\ExcelDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EF17EE-89C4-432F-9F49-7966417D2C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4DC643-D0C6-4B55-8AD8-C2DB61A3EA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00B68857-C6E1-4D98-82FE-3C4F502D76E8}"/>
+    <workbookView xWindow="-28920" yWindow="-990" windowWidth="29040" windowHeight="15840" xr2:uid="{00B68857-C6E1-4D98-82FE-3C4F502D76E8}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillTable" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>ALL</t>
   </si>
@@ -355,6 +355,26 @@
   </si>
   <si>
     <t>Skills/PoisonMist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3개의 투사체가 일정 시간마다 날아갑니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPUM/0_Flat/Icon_Flat__18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skills/SOSBullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outside</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -826,8 +846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{069061F9-1BA1-478D-A8D7-D7B6EB1F4CA2}" name="표2" displayName="표2" ref="A3:M14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A3:M14" xr:uid="{069061F9-1BA1-478D-A8D7-D7B6EB1F4CA2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{069061F9-1BA1-478D-A8D7-D7B6EB1F4CA2}" name="표2" displayName="표2" ref="A3:M15" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A3:M15" xr:uid="{069061F9-1BA1-478D-A8D7-D7B6EB1F4CA2}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{513471B3-6400-4B91-8068-618BE05D815D}" name="Index" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{CD7519DA-C7A5-4013-9D1E-02930E6F874D}" name="Name" dataDxfId="19"/>
@@ -1159,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A9E828-B25D-49C6-B4AF-221979A45248}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1679,40 +1699,40 @@
         <v>10010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="1">
         <v>1.5</v>
       </c>
       <c r="I13" s="1">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1">
         <v>12</v>
       </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
       <c r="K13" s="1">
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1720,10 +1740,10 @@
         <v>10011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>29</v>
@@ -1735,7 +1755,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="1">
         <v>1.5</v>
@@ -1750,9 +1770,50 @@
         <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>10012</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="1">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1770,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F1005-E424-4490-B83A-F7BAB1A97C24}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1852,7 +1913,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>10010</v>
+        <v>10011</v>
       </c>
       <c r="D4" s="1">
         <v>20</v>
@@ -1872,7 +1933,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="1">
-        <v>10011</v>
+        <v>10012</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>

</xml_diff>